<commit_message>
Append tabs to an existing workbook
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,10 +7,10 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Male and female populations (Metadata)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Male and female populations" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Male and female populations (Table - Percentage of male and female population in each ethnic group)" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Male and female populations (Source data)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Working age population (Metadata)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Working age population" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Working age population (Table - Percentage and number of people of working age (aged 16 to 64 years) by ethnicity)" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Working age population (Table - Percentage and number of people within each ethnic group who are of working age (aged 16 to 64 years))" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Working age population (Table - Percentage and number of people of working age (aged 16 to 64 years) by ethnicity and country)" sheetId="7" state="visible" r:id="rId7"/>

</xml_diff>